<commit_message>
ready for experimental set up: 72 models
</commit_message>
<xml_diff>
--- a/results/ablation_results.xlsx
+++ b/results/ablation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,11 +489,16 @@
           <t>F1</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Elapsed Time (seconds)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SegNet</t>
+          <t>UNet</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -510,31 +515,34 @@
         <v>16</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3700203835964203</v>
+        <v>0.4157515287399292</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7714823365567877</v>
+        <v>0.6885898578406302</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7714823365567877</v>
+        <v>0.6885898578406302</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6707322459954482</v>
+        <v>0.6265069521390475</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5479196478812542</v>
+        <v>0.4680599054620326</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8606247604079253</v>
+        <v>0.9417143419758933</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6695610204485475</v>
+        <v>0.62531816945661</v>
+      </c>
+      <c r="L2" t="n">
+        <v>25.463210105896</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SegNet</t>
+          <t>UNet</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -551,36 +559,39 @@
         <v>16</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3380044281482696</v>
+        <v>0.3847652792930603</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8401318680283315</v>
+        <v>0.7558732801111974</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8401318680283315</v>
+        <v>0.7558732801111974</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7108063239317673</v>
+        <v>0.6734722806857183</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6793537709081505</v>
+        <v>0.530768206820159</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7459615203162684</v>
+        <v>0.9160309832152219</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7111012909205385</v>
+        <v>0.6721044989539435</v>
+      </c>
+      <c r="L3" t="n">
+        <v>38.40291118621826</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SegNet</t>
+          <t>UNetPlusPlus</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CrossEntropyLoss</t>
+          <t>DiceLoss</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,72 +603,78 @@
         <v>16</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3064494371414185</v>
+        <v>0.3504891872406006</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6999358701379333</v>
+        <v>0.8474043562311319</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6184587509384448</v>
+        <v>0.8474043562311319</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7138177293997544</v>
+        <v>0.7340645515001737</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6908300748795446</v>
+        <v>0.6851525091876571</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7400194089522767</v>
+        <v>0.791167787156087</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7145792334910696</v>
+        <v>0.7343536438548353</v>
+      </c>
+      <c r="L4" t="n">
+        <v>24.62107944488525</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SegNet</t>
+          <t>UNetPlusPlus</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DiceBCELoss</t>
+          <t>DiceLoss</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Unbalanced</t>
+          <t>Balanced</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>16</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2635654658079147</v>
+        <v>0.3783090591430664</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6957633967444145</v>
+        <v>0.8471979721366559</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6148219569946967</v>
+        <v>0.8471979721366559</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7111134208165683</v>
+        <v>0.7240873391811664</v>
       </c>
       <c r="I5" t="n">
-        <v>0.6752449933301636</v>
+        <v>0.6927938548946537</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7528868423439706</v>
+        <v>0.7585855441138866</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7119553785410092</v>
+        <v>0.7241985158849915</v>
+      </c>
+      <c r="L5" t="n">
+        <v>35.12884664535522</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SegNet</t>
+          <t>UNet</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -667,73 +684,871 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Balanced</t>
+          <t>Unbalanced</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>16</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3792607486248016</v>
+        <v>0.4972993612289429</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6427694334496218</v>
+        <v>0.6366427897915597</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5683268035662512</v>
+        <v>0.5562644291143809</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6753663374827459</v>
+        <v>0.6609143752318162</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5520674184798641</v>
+        <v>0.5586919846164936</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8658699180840109</v>
+        <v>0.805471063658902</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6742449868404006</v>
+        <v>0.6597601770194005</v>
+      </c>
+      <c r="L6" t="n">
+        <v>176.6931087970734</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>UNet</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.5381702721118927</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6067517792526679</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.5358514876517445</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.6487261056900024</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.5062274304362586</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.8999636708901726</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.6479720945054618</v>
+      </c>
+      <c r="L7" t="n">
+        <v>180.7888615131378</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UNetPlusPlus</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>16</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5345514476299286</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6326163986639214</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.5597225105003072</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.6686100409581111</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.5357443392302708</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.8836657120209241</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6670643237587094</v>
+      </c>
+      <c r="L8" t="n">
+        <v>185.5482132434845</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UNet</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4.341277313232422</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.2536007140229694</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2631244117128634</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.4238374347870166</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2655800881690736</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.9923886640414289</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4190226004119524</v>
+      </c>
+      <c r="L9" t="n">
+        <v>186.8619492053986</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>UNet</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.540329599380493</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3092577070290325</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2998554329900098</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.4505869975456825</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.288376095873884</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9805796521430756</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.4456825735969039</v>
+      </c>
+      <c r="L10" t="n">
+        <v>189.221866607666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>UNetPlusPlus</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>16</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4602440357208252</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.505958064927878</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.4440376662409519</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5663280120262733</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4090243797531097</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.910275303544071</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.5644279251340028</v>
+      </c>
+      <c r="L11" t="n">
+        <v>202.2285659313202</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DiceLoss</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>16</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.4299741983413696</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6243752054689856</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.6243752054689856</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5921107576443598</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.426195353075535</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.9721587741637582</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.5925960297599209</v>
+      </c>
+      <c r="L12" t="n">
+        <v>29.54167532920837</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>UNetPlusPlus</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>16</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.5248325884342193</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5168709652700688</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.4577330556104905</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.5818698406219482</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.4161742584440301</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.9473378329161791</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5782972114556941</v>
+      </c>
+      <c r="L13" t="n">
+        <v>175.6774625778198</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DiceLoss</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>16</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.3820480048656464</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.7515621979252463</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.7515621979252463</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.6655717354554397</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.5274942662536983</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.9022295680664846</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.6657522419019004</v>
+      </c>
+      <c r="L14" t="n">
+        <v>40.64415502548218</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>SegNet</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DiceLoss</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>16</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.3700203835964203</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.7714823365567877</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.7714823365567877</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.6707322459954482</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.5479196478812542</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.8606247604079253</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.6695610204485475</v>
+      </c>
+      <c r="L15" t="n">
+        <v>15.18254590034485</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SegNet</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DiceLoss</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>16</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3380044281482696</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.8401318680283315</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8401318680283315</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.7108063239317673</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.6793537709081505</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.7459615203162684</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.7111012909205385</v>
+      </c>
+      <c r="L16" t="n">
+        <v>24.36382722854614</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>UNetPlusPlus</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>DiceBCELoss</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Balanced</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>16</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="D17" t="n">
+        <v>16</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.3305405795574188</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6951245659091421</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.6006498419756527</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.6905413361696097</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.8141695659523248</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.5993742458974771</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.6904522739719698</v>
+      </c>
+      <c r="L17" t="n">
+        <v>194.2662496566772</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.3283943176269531</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6873460550527908</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.6220055338435712</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.7265096352650569</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.5901539651714114</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.9444242109586282</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.7263959589294796</v>
+      </c>
+      <c r="L18" t="n">
+        <v>187.1358141899109</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>16</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4544160664081573</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5146501717102768</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.4608327421352388</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.5897839436164269</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4181416692213366</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.9947726194290997</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.5887913894353365</v>
+      </c>
+      <c r="L19" t="n">
+        <v>186.2620685100555</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>16</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.3832813858985901</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5901483901570181</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.5255886114525901</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.6440344590407151</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.4851168756777324</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.9565992488945148</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.6437639573977275</v>
+      </c>
+      <c r="L20" t="n">
+        <v>182.9095420837402</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>DeepLabV3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>16</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.3164457976818085</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.6852314019722632</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.621780836948258</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.7278676537367014</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.5843797493893494</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.9664304438852001</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.7283449425972242</v>
+      </c>
+      <c r="L21" t="n">
+        <v>185.2268686294556</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SegNet</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.3064494282007217</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.6999358701379333</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.6184587509384448</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.7138177293997544</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.6908300748795446</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.7400194089522767</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.7145792334910696</v>
+      </c>
+      <c r="L22" t="n">
+        <v>177.4415655136108</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SegNet</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CrossEntropyLoss</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>16</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.3799167096614838</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.6413440605918097</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.5669932857905106</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6742463386975802</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.5499698643244189</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.867222345547724</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.673086053391467</v>
+      </c>
+      <c r="L23" t="n">
+        <v>171.9320929050446</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SegNet</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Unbalanced</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2635654658079147</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.6957633967444145</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.6148219569946967</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.7111134208165683</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.6752449933301636</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.7528868423439706</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.7119553785410092</v>
+      </c>
+      <c r="L24" t="n">
+        <v>175.3385500907898</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SegNet</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DiceBCELoss</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Balanced</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>16</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.3645883202552795</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F25" t="n">
         <v>0.6953345700541678</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G25" t="n">
         <v>0.6124342020372036</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H25" t="n">
         <v>0.707936534514794</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I25" t="n">
         <v>0.6882772214890658</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J25" t="n">
         <v>0.7315064546845635</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K25" t="n">
         <v>0.7092337214194547</v>
+      </c>
+      <c r="L25" t="n">
+        <v>188.7168519496918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>